<commit_message>
New files received from WRI 4/13/2020
</commit_message>
<xml_diff>
--- a/InputData/trans/SDoVPbT/Std Dev of Veh Prices by Technology.xlsx
+++ b/InputData/trans/SDoVPbT/Std Dev of Veh Prices by Technology.xlsx
@@ -17,13 +17,14 @@
     <sheet name="Conventional Daycab Trucks" sheetId="5" r:id="rId3"/>
     <sheet name="Conventional Sleeper Trucks" sheetId="6" r:id="rId4"/>
     <sheet name="Motorbikes" sheetId="8" r:id="rId5"/>
-    <sheet name="Calculations" sheetId="7" r:id="rId6"/>
-    <sheet name="Data from BNVP" sheetId="9" r:id="rId7"/>
-    <sheet name="SDoVPbT-psgr" sheetId="2" r:id="rId8"/>
-    <sheet name="SDoVPbT-frgt" sheetId="4" r:id="rId9"/>
+    <sheet name="Freight Motorbikes - India" sheetId="11" r:id="rId6"/>
+    <sheet name="Calculations" sheetId="7" r:id="rId7"/>
+    <sheet name="Data from BNVP" sheetId="9" r:id="rId8"/>
+    <sheet name="SDoVPbT-psgr" sheetId="2" r:id="rId9"/>
+    <sheet name="SDoVPbT-frgt" sheetId="4" r:id="rId10"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId11"/>
   </externalReferences>
   <definedNames>
     <definedName name="cpi_2010to2012">[1]About!#REF!</definedName>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="631">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1213" uniqueCount="663">
   <si>
     <t>SDoVPbT Standard Dev of Vehicle Prices by Technology</t>
   </si>
@@ -1459,15 +1460,9 @@
     <t>Standard Deviation</t>
   </si>
   <si>
-    <t>Units</t>
-  </si>
-  <si>
     <t>freight HDVs</t>
   </si>
   <si>
-    <t>$</t>
-  </si>
-  <si>
     <t>Example New 2017 Motorcycles Selected by Popular Mechanics Magazine (U.S. market)</t>
   </si>
   <si>
@@ -1933,21 +1928,124 @@
     <t>While India-specific prices are available used for the BNVP variable, we find that</t>
   </si>
   <si>
-    <t>measure may not be meaningful. Hence, we use the US values. US assumptions:</t>
-  </si>
-  <si>
     <t>the sample size is limited to a few for each type due to which the standard deviation</t>
+  </si>
+  <si>
+    <t>Fuel Type</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Bajaj RE Maxima</t>
+  </si>
+  <si>
+    <t>Diesel</t>
+  </si>
+  <si>
+    <t>lakhs</t>
+  </si>
+  <si>
+    <t>Bajaj RE Optima CNG Auto Rickshaw</t>
+  </si>
+  <si>
+    <t>CNG</t>
+  </si>
+  <si>
+    <t>Atul Gemini Petrol Auto Rickshaw</t>
+  </si>
+  <si>
+    <t>Gasoline</t>
+  </si>
+  <si>
+    <t>Atul Gemini CNG Auto Rickshaw</t>
+  </si>
+  <si>
+    <t>Atul Gemini LPG Auto Rickshaw</t>
+  </si>
+  <si>
+    <t>LPG</t>
+  </si>
+  <si>
+    <t>Lohia Auto Humsafar Diesel Auto Rickshaw</t>
+  </si>
+  <si>
+    <t>HERO Raahii Electric Rickshaw</t>
+  </si>
+  <si>
+    <t>Electricity</t>
+  </si>
+  <si>
+    <t>Piaggio Ape City Smart CNG, LPG, or Petrol</t>
+  </si>
+  <si>
+    <t>CNG, LPG</t>
+  </si>
+  <si>
+    <t>Piaggio Ape City Smart Diesel</t>
+  </si>
+  <si>
+    <t>Mahindra Alfa DX</t>
+  </si>
+  <si>
+    <t>Mahindra eAlfa Mini Electric Rickshaw</t>
+  </si>
+  <si>
+    <t>from trans/BNVP - EPS India 2.1</t>
+  </si>
+  <si>
+    <t>freight motorbikes</t>
+  </si>
+  <si>
+    <t>US assumptions:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">measure may not be meaningful. Hence, we use the US values for all vehicle types </t>
+  </si>
+  <si>
+    <t xml:space="preserve">except freight motorbikes. </t>
+  </si>
+  <si>
+    <t>India freight motorbikes:</t>
+  </si>
+  <si>
+    <t>Freight motorbikes are considered as 3-wheelers (autorickshaws) in the India model.</t>
+  </si>
+  <si>
+    <t>Price range is taken from trans/BNVP variable from EPS-India 2.1.0</t>
+  </si>
+  <si>
+    <t>See trans/BNVP variable - tab 'Freight Motorbikes - India'</t>
+  </si>
+  <si>
+    <t>Price (US $)</t>
+  </si>
+  <si>
+    <t>Ruppees per Lakh</t>
+  </si>
+  <si>
+    <t>We convert to 2012 USD, the currency input unit for the model.</t>
+  </si>
+  <si>
+    <t>We convert back to Indian currency in the model's output area.</t>
+  </si>
+  <si>
+    <t>(See "scaling-factors.xlsx" for source info)</t>
+  </si>
+  <si>
+    <t>Ruppees per dollar</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2003,6 +2101,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -2098,7 +2204,7 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2147,6 +2253,13 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Body: normal cell" xfId="2"/>
@@ -2525,15 +2638,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B67"/>
+  <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="2" max="2" width="64.73046875" customWidth="1"/>
+    <col min="5" max="5" width="56.86328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.45">
@@ -2546,12 +2658,12 @@
         <v>1</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B4" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.45">
@@ -2561,198 +2673,206 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B6" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B7" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B9" s="6" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B10" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B11" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B12" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B13" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B14" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B15" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.45">
       <c r="B16" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="20" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="21" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="22" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B22" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="23" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B23" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="24" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B24" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="25" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B25" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="26" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="28" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B28" s="6" t="s">
-        <v>504</v>
+        <v>502</v>
       </c>
     </row>
     <row r="29" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B29" t="s">
-        <v>499</v>
+        <v>497</v>
       </c>
     </row>
     <row r="30" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B30" t="s">
-        <v>500</v>
+        <v>498</v>
       </c>
     </row>
     <row r="31" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B31" t="s">
-        <v>501</v>
+        <v>499</v>
       </c>
     </row>
     <row r="32" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B32" s="8" t="s">
-        <v>502</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B33" s="8" t="s">
-        <v>503</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B35" s="11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+        <v>496</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B36" s="9" t="s">
-        <v>521</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+        <v>519</v>
+      </c>
+      <c r="E36" s="25" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B37" s="12">
         <v>2016</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B38" s="9" t="s">
-        <v>522</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B39" s="10" t="s">
-        <v>523</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A45" s="1"/>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A45" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A46" s="1" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A47" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
-      <c r="A47" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.45">
@@ -2762,84 +2882,421 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>618</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A52" s="1" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A51" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A53" s="1" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A53" t="s">
-        <v>505</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A54" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A55" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A56" t="s">
-        <v>508</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A58" s="1" t="s">
-        <v>13</v>
+        <v>505</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A57" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A59" t="s">
-        <v>525</v>
+      <c r="A59" s="1" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A60" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A61" t="s">
-        <v>507</v>
+        <v>522</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A62" t="s">
-        <v>526</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A64" s="1" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A65" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.45">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.45">
+      <c r="A63" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A65" s="1" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A66" t="s">
         <v>625</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A67" t="s">
-        <v>626</v>
-      </c>
+        <v>623</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A68" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A70" s="1" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A71" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A72" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A74" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A75" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A76" s="28" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A77" s="1" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A78">
+        <v>54.77</v>
+      </c>
+      <c r="B78" s="13">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A80" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="C80" s="8"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A81">
+        <v>100000</v>
+      </c>
+      <c r="B81" s="2"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B82" s="26"/>
+      <c r="C82" s="24"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B83" s="26"/>
+      <c r="C83" s="24"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B84" s="26"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B85" s="26"/>
+      <c r="C85" s="24"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B86" s="26"/>
+      <c r="C86" s="24"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B87" s="26"/>
+      <c r="C87" s="24"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B88" s="26"/>
+      <c r="C88" s="24"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B89" s="27"/>
+      <c r="C89" s="24"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B90" s="26"/>
+      <c r="C90" s="24"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="B91" s="26"/>
+      <c r="C91" s="24"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B33" r:id="rId1"/>
     <hyperlink ref="B32" r:id="rId2"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="3"/>
+  </sheetPr>
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15.3984375" customWidth="1"/>
+    <col min="2" max="3" width="24.265625" customWidth="1"/>
+    <col min="4" max="4" width="18.73046875" customWidth="1"/>
+    <col min="5" max="5" width="17.73046875" customWidth="1"/>
+    <col min="6" max="8" width="24.265625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="19" t="s">
+        <v>621</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>619</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="3">
+        <f>'SDoVPbT-psgr'!D2*('Data from BNVP'!C2/'Data from BNVP'!B4)</f>
+        <v>21663.926762859195</v>
+      </c>
+      <c r="C2" s="3">
+        <f>'SDoVPbT-psgr'!D2*('Data from BNVP'!C3/'Data from BNVP'!B4)</f>
+        <v>17550.150350913391</v>
+      </c>
+      <c r="D2" s="3">
+        <f>'SDoVPbT-psgr'!D2*('Data from BNVP'!C4/'Data from BNVP'!B4)</f>
+        <v>15703.80001929629</v>
+      </c>
+      <c r="E2" s="3">
+        <f>'SDoVPbT-psgr'!D2*('Data from BNVP'!C5/'Data from BNVP'!B4)</f>
+        <v>17228.81329081468</v>
+      </c>
+      <c r="F2" s="3">
+        <f>'SDoVPbT-psgr'!D2*('Data from BNVP'!C6/'Data from BNVP'!B4)</f>
+        <v>14738.77305885482</v>
+      </c>
+      <c r="G2" s="3">
+        <f>'SDoVPbT-psgr'!D2*('Data from BNVP'!C7/'Data from BNVP'!B4)</f>
+        <v>19508.539203654229</v>
+      </c>
+      <c r="H2" s="3">
+        <f>'SDoVPbT-psgr'!D2*('Data from BNVP'!C8/'Data from BNVP'!B4)</f>
+        <v>22143.359548864228</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="3">
+        <f>E3*('Data from BNVP'!E2/'Data from BNVP'!E5)</f>
+        <v>21135.933029022086</v>
+      </c>
+      <c r="C3" s="3">
+        <f>E3*('Data from BNVP'!E3/'Data from BNVP'!E5)</f>
+        <v>13884.41947332269</v>
+      </c>
+      <c r="D3" s="3">
+        <f>E3*('Data from BNVP'!E4/'Data from BNVP'!E5)</f>
+        <v>13630.200652086061</v>
+      </c>
+      <c r="E3" s="18">
+        <f>Calculations!B3</f>
+        <v>13630.200652086061</v>
+      </c>
+      <c r="F3" s="3">
+        <f>E3*('Data from BNVP'!E6/'Data from BNVP'!E5)</f>
+        <v>15832.321026872658</v>
+      </c>
+      <c r="G3" s="3">
+        <f>E3*('Data from BNVP'!E7/'Data from BNVP'!E5)</f>
+        <v>15433.756190082944</v>
+      </c>
+      <c r="H3" s="3">
+        <f>E3*('Data from BNVP'!E8/'Data from BNVP'!E5)</f>
+        <v>17518.236959664304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="3">
+        <f>$E$3*('Data from BNVP'!G2/'Data from BNVP'!$E$5)</f>
+        <v>9734270.8443508428</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3">
+        <f>$E$3*('Data from BNVP'!G5/'Data from BNVP'!$E$5)</f>
+        <v>6647893.9232045906</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="3">
+        <f>$E$3*('Data from BNVP'!G8/'Data from BNVP'!$E$5)</f>
+        <v>15428147.692604657</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3">
+        <f>$E$3*('Data from BNVP'!I2/'Data from BNVP'!$E$5)</f>
+        <v>375357.48757136922</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <f>$E$3*('Data from BNVP'!I5/'Data from BNVP'!$E$5)</f>
+        <v>256345.52403102536</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="3">
+        <f>$E$3*('Data from BNVP'!I8/'Data from BNVP'!$E$5)</f>
+        <v>594915.72079452395</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="3">
+        <f>$E$3*('Data from BNVP'!K2/'Data from BNVP'!$E$5)</f>
+        <v>1501429.9502854769</v>
+      </c>
+      <c r="C6" s="3">
+        <v>0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <f>$E$3*('Data from BNVP'!K5/'Data from BNVP'!$E$5)</f>
+        <v>1025382.0961241014</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" s="3">
+        <f>$E$3*('Data from BNVP'!K8/'Data from BNVP'!$E$5)</f>
+        <v>2379662.8831780958</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3">
+        <f>Calculations!B5</f>
+        <v>787.55347823519639</v>
+      </c>
+      <c r="C7" s="3">
+        <f>B7</f>
+        <v>787.55347823519639</v>
+      </c>
+      <c r="D7" s="3">
+        <f>C7</f>
+        <v>787.55347823519639</v>
+      </c>
+      <c r="E7" s="3">
+        <f>D7</f>
+        <v>787.55347823519639</v>
+      </c>
+      <c r="F7" s="3">
+        <f>D7</f>
+        <v>787.55347823519639</v>
+      </c>
+      <c r="G7" s="3">
+        <f>E7</f>
+        <v>787.55347823519639</v>
+      </c>
+      <c r="H7" s="3">
+        <f>D7</f>
+        <v>787.55347823519639</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2848,7 +3305,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -2859,24 +3318,24 @@
   <sheetData>
     <row r="1" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="14" t="s">
-        <v>475</v>
+        <v>473</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="C1" s="15" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B2" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -2887,10 +3346,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B3" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -2901,10 +3360,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B4" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -2915,10 +3374,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B5" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="C5">
         <v>4</v>
@@ -2929,10 +3388,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B6" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="C6">
         <v>5</v>
@@ -2943,10 +3402,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
+        <v>533</v>
+      </c>
+      <c r="B7" t="s">
         <v>535</v>
-      </c>
-      <c r="B7" t="s">
-        <v>537</v>
       </c>
       <c r="C7">
         <v>6</v>
@@ -2957,10 +3416,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B8" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="C8">
         <v>7</v>
@@ -2971,10 +3430,10 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B9" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -2985,10 +3444,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B10" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="C10">
         <v>9</v>
@@ -2999,10 +3458,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B11" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="C11">
         <v>10</v>
@@ -3013,10 +3472,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B12" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="C12">
         <v>11</v>
@@ -3027,10 +3486,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B13" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="C13">
         <v>12</v>
@@ -3041,10 +3500,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B14" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="C14">
         <v>13</v>
@@ -3055,10 +3514,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="B15" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
       <c r="C15">
         <v>14</v>
@@ -3069,10 +3528,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B16" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
       <c r="C16">
         <v>15</v>
@@ -3083,10 +3542,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B17" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -3097,10 +3556,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B18" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="C18">
         <v>17</v>
@@ -3111,10 +3570,10 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B19" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C19">
         <v>18</v>
@@ -3125,10 +3584,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B20" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="C20">
         <v>19</v>
@@ -3139,10 +3598,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="B21" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="C21">
         <v>20</v>
@@ -3153,10 +3612,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B22" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="C22">
         <v>21</v>
@@ -3167,10 +3626,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B23" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="C23">
         <v>22</v>
@@ -3181,10 +3640,10 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B24" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C24">
         <v>23</v>
@@ -3195,10 +3654,10 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="B25" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="C25">
         <v>24</v>
@@ -3209,10 +3668,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
       <c r="B26" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="C26">
         <v>25</v>
@@ -3223,10 +3682,10 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="B27" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="C27">
         <v>26</v>
@@ -3237,10 +3696,10 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B28" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C28">
         <v>27</v>
@@ -3251,10 +3710,10 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A29" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B29" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="C29">
         <v>28</v>
@@ -3265,10 +3724,10 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B30" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="C30">
         <v>29</v>
@@ -3279,10 +3738,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="B31" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="C31">
         <v>30</v>
@@ -3293,10 +3752,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B32" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="C32">
         <v>31</v>
@@ -3307,10 +3766,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B33" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="C33">
         <v>32</v>
@@ -3321,10 +3780,10 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B34" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="C34">
         <v>33</v>
@@ -3335,7 +3794,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A35" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="B35" s="13">
         <v>1500</v>
@@ -3349,10 +3808,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A36" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B36" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
       <c r="C36">
         <v>35</v>
@@ -3363,10 +3822,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A37" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B37" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
       <c r="C37">
         <v>36</v>
@@ -3377,7 +3836,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A38" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="B38" s="13">
         <v>3</v>
@@ -3391,10 +3850,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A39" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B39" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="C39">
         <v>38</v>
@@ -3405,10 +3864,10 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A40" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B40" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
       <c r="C40">
         <v>39</v>
@@ -3419,10 +3878,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A41" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B41" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
       <c r="C41">
         <v>40</v>
@@ -3433,10 +3892,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A42" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="B42" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
       <c r="C42">
         <v>41</v>
@@ -3447,10 +3906,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A43" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="B43" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C43">
         <v>42</v>
@@ -3461,10 +3920,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A44" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B44" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
       <c r="C44">
         <v>43</v>
@@ -3475,10 +3934,10 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A45" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="B45" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="C45">
         <v>44</v>
@@ -3489,10 +3948,10 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A46" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="B46" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="C46">
         <v>45</v>
@@ -3503,10 +3962,10 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A47" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B47" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C47">
         <v>46</v>
@@ -3517,10 +3976,10 @@
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A48" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="B48" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C48">
         <v>47</v>
@@ -3531,10 +3990,10 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A49" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B49" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C49">
         <v>48</v>
@@ -3545,10 +4004,10 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A50" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="B50" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C50">
         <v>49</v>
@@ -3559,10 +4018,10 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A51" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="B51" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C51">
         <v>50</v>
@@ -8688,7 +9147,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -8698,26 +9159,26 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>474</v>
+        <v>472</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="6" t="s">
+        <v>473</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>474</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>475</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>476</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>477</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>478</v>
+        <v>476</v>
       </c>
       <c r="B3" t="s">
-        <v>479</v>
+        <v>477</v>
       </c>
       <c r="C3">
         <v>8700</v>
@@ -8725,10 +9186,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>480</v>
+        <v>478</v>
       </c>
       <c r="B4" t="s">
-        <v>481</v>
+        <v>479</v>
       </c>
       <c r="C4">
         <v>4600</v>
@@ -8736,10 +9197,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="B5" t="s">
-        <v>483</v>
+        <v>481</v>
       </c>
       <c r="C5">
         <v>10500</v>
@@ -8747,10 +9208,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>484</v>
+        <v>482</v>
       </c>
       <c r="B6" t="s">
-        <v>485</v>
+        <v>483</v>
       </c>
       <c r="C6">
         <v>6500</v>
@@ -8758,10 +9219,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>486</v>
+        <v>484</v>
       </c>
       <c r="B7" t="s">
-        <v>487</v>
+        <v>485</v>
       </c>
       <c r="C7">
         <v>3000</v>
@@ -8769,10 +9230,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>488</v>
+        <v>486</v>
       </c>
       <c r="B8" t="s">
-        <v>489</v>
+        <v>487</v>
       </c>
       <c r="C8">
         <v>10000</v>
@@ -8780,10 +9241,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>490</v>
+        <v>488</v>
       </c>
       <c r="B9" t="s">
-        <v>491</v>
+        <v>489</v>
       </c>
       <c r="C9">
         <v>13000</v>
@@ -8791,10 +9252,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>492</v>
+        <v>490</v>
       </c>
       <c r="B10" t="s">
-        <v>493</v>
+        <v>491</v>
       </c>
       <c r="C10">
         <v>9000</v>
@@ -8802,10 +9263,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>494</v>
+        <v>492</v>
       </c>
       <c r="B11" t="s">
-        <v>495</v>
+        <v>493</v>
       </c>
       <c r="C11">
         <v>19000</v>
@@ -8813,10 +9274,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>496</v>
+        <v>494</v>
       </c>
       <c r="B12" t="s">
-        <v>497</v>
+        <v>495</v>
       </c>
       <c r="C12">
         <v>5500</v>
@@ -8829,9 +9290,269 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="38.73046875" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>628</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>630</v>
+      </c>
+      <c r="B2" t="s">
+        <v>631</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>632</v>
+      </c>
+      <c r="E2">
+        <f>C2*About!$A$81/About!$A$78</f>
+        <v>3651.6341062625525</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>633</v>
+      </c>
+      <c r="B3" t="s">
+        <v>634</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>632</v>
+      </c>
+      <c r="E3">
+        <f>C3*About!$A$81/About!$A$78</f>
+        <v>3651.6341062625525</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>635</v>
+      </c>
+      <c r="B4" t="s">
+        <v>636</v>
+      </c>
+      <c r="C4">
+        <v>2.1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>632</v>
+      </c>
+      <c r="E4">
+        <f>C4*About!$A$81/About!$A$78</f>
+        <v>3834.2158115756797</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>637</v>
+      </c>
+      <c r="B5" t="s">
+        <v>634</v>
+      </c>
+      <c r="C5">
+        <v>2.15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>632</v>
+      </c>
+      <c r="E5">
+        <f>C5*About!$A$81/About!$A$78</f>
+        <v>3925.5066642322436</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>638</v>
+      </c>
+      <c r="B6" t="s">
+        <v>639</v>
+      </c>
+      <c r="C6">
+        <v>2.5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>632</v>
+      </c>
+      <c r="E6">
+        <f>C6*About!$A$81/About!$A$78</f>
+        <v>4564.5426328281901</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>640</v>
+      </c>
+      <c r="B7" t="s">
+        <v>631</v>
+      </c>
+      <c r="C7">
+        <v>1.3</v>
+      </c>
+      <c r="D7" t="s">
+        <v>632</v>
+      </c>
+      <c r="E7">
+        <f>C7*About!$A$81/About!$A$78</f>
+        <v>2373.5621690706589</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>641</v>
+      </c>
+      <c r="B8" t="s">
+        <v>642</v>
+      </c>
+      <c r="C8">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D8" t="s">
+        <v>632</v>
+      </c>
+      <c r="E8">
+        <f>C8*About!$A$81/About!$A$78</f>
+        <v>2008.3987584444039</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>643</v>
+      </c>
+      <c r="B9" t="s">
+        <v>644</v>
+      </c>
+      <c r="C9">
+        <v>1.75</v>
+      </c>
+      <c r="D9" t="s">
+        <v>632</v>
+      </c>
+      <c r="E9">
+        <f>C9*About!$A$81/About!$A$78</f>
+        <v>3195.1798429797332</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>643</v>
+      </c>
+      <c r="B10" t="s">
+        <v>636</v>
+      </c>
+      <c r="C10">
+        <v>1.75</v>
+      </c>
+      <c r="D10" t="s">
+        <v>632</v>
+      </c>
+      <c r="E10">
+        <f>C10*About!$A$81/About!$A$78</f>
+        <v>3195.1798429797332</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>645</v>
+      </c>
+      <c r="B11" t="s">
+        <v>631</v>
+      </c>
+      <c r="C11">
+        <v>1.8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>632</v>
+      </c>
+      <c r="E11">
+        <f>C11*About!$A$81/About!$A$78</f>
+        <v>3286.470695636297</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>646</v>
+      </c>
+      <c r="B12" t="s">
+        <v>631</v>
+      </c>
+      <c r="C12">
+        <v>1.52</v>
+      </c>
+      <c r="D12" t="s">
+        <v>632</v>
+      </c>
+      <c r="E12">
+        <f>C12*About!$A$81/About!$A$78</f>
+        <v>2775.2419207595399</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>647</v>
+      </c>
+      <c r="B13" t="s">
+        <v>642</v>
+      </c>
+      <c r="C13">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="D13" t="s">
+        <v>632</v>
+      </c>
+      <c r="E13">
+        <f>C13*About!$A$81/About!$A$78</f>
+        <v>2044.9150995070295</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>648</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
@@ -8839,51 +9560,48 @@
     <col min="2" max="2" width="25.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="6" t="s">
         <v>469</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>470</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
       <c r="B2" s="17">
         <f>_xlfn.STDEV.S(LDVs!D2:D51)</f>
         <v>8309.8800311829455</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B3" s="3">
         <f>_xlfn.STDEV.S('Conventional Daycab Trucks'!C:C,'Conventional Sleeper Trucks'!C:C)</f>
         <v>13630.200652086061</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>473</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>498</v>
+        <v>496</v>
       </c>
       <c r="B4" s="3">
         <f>_xlfn.STDEV.S(Motorbikes!C3:C12)</f>
         <v>4633.1654645849012</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>473</v>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>649</v>
+      </c>
+      <c r="B5" s="3">
+        <f>_xlfn.STDEV.S('Freight Motorbikes - India'!E2:E13)</f>
+        <v>787.55347823519639</v>
       </c>
     </row>
   </sheetData>
@@ -8892,7 +9610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M8"/>
   <sheetViews>
@@ -8909,43 +9627,43 @@
   <sheetData>
     <row r="1" spans="1:13" s="2" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="23" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="B1" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="D1" s="22" t="s">
         <v>509</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="E1" s="22" t="s">
         <v>510</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="F1" s="22" t="s">
         <v>511</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="G1" s="22" t="s">
         <v>512</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="H1" s="22" t="s">
         <v>513</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="I1" s="22" t="s">
         <v>514</v>
       </c>
-      <c r="H1" s="22" t="s">
+      <c r="J1" s="22" t="s">
         <v>515</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="K1" s="22" t="s">
         <v>516</v>
       </c>
-      <c r="J1" s="22" t="s">
+      <c r="L1" s="22" t="s">
         <v>517</v>
       </c>
-      <c r="K1" s="22" t="s">
+      <c r="M1" s="22" t="s">
         <v>518</v>
-      </c>
-      <c r="L1" s="22" t="s">
-        <v>519</v>
-      </c>
-      <c r="M1" s="22" t="s">
-        <v>520</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.45">
@@ -9155,7 +9873,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7" s="1" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B7" s="3">
         <v>39464.208493999999</v>
@@ -9196,7 +9914,7 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="B8" s="3">
         <v>71671.802858802301</v>
@@ -9238,237 +9956,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr>
-    <tabColor theme="3"/>
-  </sheetPr>
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="15.3984375" customWidth="1"/>
-    <col min="2" max="3" width="24.265625" customWidth="1"/>
-    <col min="4" max="4" width="18.73046875" customWidth="1"/>
-    <col min="5" max="5" width="17.73046875" customWidth="1"/>
-    <col min="6" max="8" width="24.265625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="19" t="s">
-        <v>623</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>621</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="3">
-        <f>D2*('Data from BNVP'!B2/'Data from BNVP'!B4)</f>
-        <v>13658.022529814965</v>
-      </c>
-      <c r="C2" s="3">
-        <f>D2*('Data from BNVP'!B3/'Data from BNVP'!B4)</f>
-        <v>10302.330516464528</v>
-      </c>
-      <c r="D2" s="18">
-        <f>Calculations!B2</f>
-        <v>8309.8800311829455</v>
-      </c>
-      <c r="E2" s="3">
-        <f>D2*('Data from BNVP'!B5/'Data from BNVP'!B4)</f>
-        <v>8807.824444583006</v>
-      </c>
-      <c r="F2" s="3">
-        <f>D2*('Data from BNVP'!B6/'Data from BNVP'!B4)</f>
-        <v>10230.832818563998</v>
-      </c>
-      <c r="G2" s="3">
-        <f>D2*('Data from BNVP'!B7/'Data from BNVP'!B4)</f>
-        <v>10618.899938992296</v>
-      </c>
-      <c r="H2" s="3">
-        <f>D2*('Data from BNVP'!B8/'Data from BNVP'!B4)</f>
-        <v>19285.213920368249</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="3">
-        <f>'SDoVPbT-frgt'!E$3*('Data from BNVP'!D2/'Data from BNVP'!$E$5)</f>
-        <v>72164.341161022006</v>
-      </c>
-      <c r="C3" s="3">
-        <f>'SDoVPbT-frgt'!E3*('Data from BNVP'!D3/'Data from BNVP'!E5)</f>
-        <v>50202.897446801551</v>
-      </c>
-      <c r="D3" s="3">
-        <f>'SDoVPbT-frgt'!E3*('Data from BNVP'!D4/'Data from BNVP'!E5)</f>
-        <v>49283.700109375168</v>
-      </c>
-      <c r="E3" s="3">
-        <f>'SDoVPbT-frgt'!E3*('Data from BNVP'!D5/'Data from BNVP'!E5)</f>
-        <v>49283.700109375168</v>
-      </c>
-      <c r="F3" s="3">
-        <f>'SDoVPbT-frgt'!E3*('Data from BNVP'!D6/'Data from BNVP'!E5)</f>
-        <v>57246.065662601075</v>
-      </c>
-      <c r="G3" s="3">
-        <f>'SDoVPbT-frgt'!E3*('Data from BNVP'!D7/'Data from BNVP'!E5)</f>
-        <v>62977.886337819873</v>
-      </c>
-      <c r="H3" s="3">
-        <f>'SDoVPbT-frgt'!E3*('Data from BNVP'!D8/'Data from BNVP'!E5)</f>
-        <v>114375.50191218297</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="3">
-        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!F2/'Data from BNVP'!$E$5)</f>
-        <v>9734270.8443508428</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3">
-        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!F5/'Data from BNVP'!$E$5)</f>
-        <v>6647893.9232045906</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
-        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!F8/'Data from BNVP'!$E$5)</f>
-        <v>15428147.692604657</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="3">
-        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!H2/'Data from BNVP'!$E$5)</f>
-        <v>375357.48757136922</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3">
-        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!H5/'Data from BNVP'!$E$5)</f>
-        <v>256345.52403102536</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
-        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!H8/'Data from BNVP'!$E$5)</f>
-        <v>594915.72079452395</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="3">
-        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!J2/'Data from BNVP'!$E$5)</f>
-        <v>4504.2898508564313</v>
-      </c>
-      <c r="C6" s="3">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3">
-        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!J4/'Data from BNVP'!$E$5)</f>
-        <v>3076.1462883723043</v>
-      </c>
-      <c r="E6" s="3">
-        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!J5/'Data from BNVP'!$E$5)</f>
-        <v>3076.1462883723043</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
-        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!J8/'Data from BNVP'!$E$5)</f>
-        <v>7138.988649534288</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" s="3">
-        <f>D7*('Data from BNVP'!L2/'Data from BNVP'!L4)</f>
-        <v>7615.0170715103632</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" s="18">
-        <f>Calculations!B4</f>
-        <v>4633.1654645849012</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -9479,8 +9966,8 @@
   </sheetPr>
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9494,7 +9981,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A1" s="19" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>3</v>
@@ -9512,10 +9999,10 @@
         <v>7</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.45">
@@ -9523,32 +10010,32 @@
         <v>8</v>
       </c>
       <c r="B2" s="3">
-        <f>'SDoVPbT-psgr'!D2*('Data from BNVP'!C2/'Data from BNVP'!B4)</f>
-        <v>21663.926762859195</v>
+        <f>D2*('Data from BNVP'!B2/'Data from BNVP'!B4)</f>
+        <v>13658.022529814965</v>
       </c>
       <c r="C2" s="3">
-        <f>'SDoVPbT-psgr'!D2*('Data from BNVP'!C3/'Data from BNVP'!B4)</f>
-        <v>17550.150350913391</v>
-      </c>
-      <c r="D2" s="3">
-        <f>'SDoVPbT-psgr'!D2*('Data from BNVP'!C4/'Data from BNVP'!B4)</f>
-        <v>15703.80001929629</v>
+        <f>D2*('Data from BNVP'!B3/'Data from BNVP'!B4)</f>
+        <v>10302.330516464528</v>
+      </c>
+      <c r="D2" s="18">
+        <f>Calculations!B2</f>
+        <v>8309.8800311829455</v>
       </c>
       <c r="E2" s="3">
-        <f>'SDoVPbT-psgr'!D2*('Data from BNVP'!C5/'Data from BNVP'!B4)</f>
-        <v>17228.81329081468</v>
+        <f>D2*('Data from BNVP'!B5/'Data from BNVP'!B4)</f>
+        <v>8807.824444583006</v>
       </c>
       <c r="F2" s="3">
-        <f>'SDoVPbT-psgr'!D2*('Data from BNVP'!C6/'Data from BNVP'!B4)</f>
-        <v>14738.77305885482</v>
+        <f>D2*('Data from BNVP'!B6/'Data from BNVP'!B4)</f>
+        <v>10230.832818563998</v>
       </c>
       <c r="G2" s="3">
-        <f>'SDoVPbT-psgr'!D2*('Data from BNVP'!C7/'Data from BNVP'!B4)</f>
-        <v>19508.539203654229</v>
+        <f>D2*('Data from BNVP'!B7/'Data from BNVP'!B4)</f>
+        <v>10618.899938992296</v>
       </c>
       <c r="H2" s="3">
-        <f>'SDoVPbT-psgr'!D2*('Data from BNVP'!C8/'Data from BNVP'!B4)</f>
-        <v>22143.359548864228</v>
+        <f>D2*('Data from BNVP'!B8/'Data from BNVP'!B4)</f>
+        <v>19285.213920368249</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.45">
@@ -9556,32 +10043,32 @@
         <v>9</v>
       </c>
       <c r="B3" s="3">
-        <f>E3*('Data from BNVP'!E2/'Data from BNVP'!E5)</f>
-        <v>21135.933029022086</v>
+        <f>'SDoVPbT-frgt'!E$3*('Data from BNVP'!D2/'Data from BNVP'!$E$5)</f>
+        <v>72164.341161022006</v>
       </c>
       <c r="C3" s="3">
-        <f>E3*('Data from BNVP'!E3/'Data from BNVP'!E5)</f>
-        <v>13884.41947332269</v>
+        <f>'SDoVPbT-frgt'!E3*('Data from BNVP'!D3/'Data from BNVP'!E5)</f>
+        <v>50202.897446801551</v>
       </c>
       <c r="D3" s="3">
-        <f>E3*('Data from BNVP'!E4/'Data from BNVP'!E5)</f>
-        <v>13630.200652086061</v>
-      </c>
-      <c r="E3" s="18">
-        <f>Calculations!B3</f>
-        <v>13630.200652086061</v>
+        <f>'SDoVPbT-frgt'!E3*('Data from BNVP'!D4/'Data from BNVP'!E5)</f>
+        <v>49283.700109375168</v>
+      </c>
+      <c r="E3" s="3">
+        <f>'SDoVPbT-frgt'!E3*('Data from BNVP'!D5/'Data from BNVP'!E5)</f>
+        <v>49283.700109375168</v>
       </c>
       <c r="F3" s="3">
-        <f>E3*('Data from BNVP'!E6/'Data from BNVP'!E5)</f>
-        <v>15832.321026872658</v>
+        <f>'SDoVPbT-frgt'!E3*('Data from BNVP'!D6/'Data from BNVP'!E5)</f>
+        <v>57246.065662601075</v>
       </c>
       <c r="G3" s="3">
-        <f>E3*('Data from BNVP'!E7/'Data from BNVP'!E5)</f>
-        <v>15433.756190082944</v>
+        <f>'SDoVPbT-frgt'!E3*('Data from BNVP'!D7/'Data from BNVP'!E5)</f>
+        <v>62977.886337819873</v>
       </c>
       <c r="H3" s="3">
-        <f>E3*('Data from BNVP'!E8/'Data from BNVP'!E5)</f>
-        <v>17518.236959664304</v>
+        <f>'SDoVPbT-frgt'!E3*('Data from BNVP'!D8/'Data from BNVP'!E5)</f>
+        <v>114375.50191218297</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.45">
@@ -9589,7 +10076,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="3">
-        <f>$E$3*('Data from BNVP'!G2/'Data from BNVP'!$E$5)</f>
+        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!F2/'Data from BNVP'!$E$5)</f>
         <v>9734270.8443508428</v>
       </c>
       <c r="C4" s="3">
@@ -9599,7 +10086,7 @@
         <v>0</v>
       </c>
       <c r="E4" s="3">
-        <f>$E$3*('Data from BNVP'!G5/'Data from BNVP'!$E$5)</f>
+        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!F5/'Data from BNVP'!$E$5)</f>
         <v>6647893.9232045906</v>
       </c>
       <c r="F4">
@@ -9609,7 +10096,7 @@
         <v>0</v>
       </c>
       <c r="H4" s="3">
-        <f>$E$3*('Data from BNVP'!G8/'Data from BNVP'!$E$5)</f>
+        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!F8/'Data from BNVP'!$E$5)</f>
         <v>15428147.692604657</v>
       </c>
     </row>
@@ -9618,7 +10105,7 @@
         <v>11</v>
       </c>
       <c r="B5" s="3">
-        <f>$E$3*('Data from BNVP'!I2/'Data from BNVP'!$E$5)</f>
+        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!H2/'Data from BNVP'!$E$5)</f>
         <v>375357.48757136922</v>
       </c>
       <c r="C5" s="3">
@@ -9628,7 +10115,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="3">
-        <f>$E$3*('Data from BNVP'!I5/'Data from BNVP'!$E$5)</f>
+        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!H5/'Data from BNVP'!$E$5)</f>
         <v>256345.52403102536</v>
       </c>
       <c r="F5">
@@ -9638,7 +10125,7 @@
         <v>0</v>
       </c>
       <c r="H5" s="3">
-        <f>$E$3*('Data from BNVP'!I8/'Data from BNVP'!$E$5)</f>
+        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!H8/'Data from BNVP'!$E$5)</f>
         <v>594915.72079452395</v>
       </c>
     </row>
@@ -9647,18 +10134,19 @@
         <v>12</v>
       </c>
       <c r="B6" s="3">
-        <f>$E$3*('Data from BNVP'!K2/'Data from BNVP'!$E$5)</f>
-        <v>1501429.9502854769</v>
+        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!J2/'Data from BNVP'!$E$5)</f>
+        <v>4504.2898508564313</v>
       </c>
       <c r="C6" s="3">
         <v>0</v>
       </c>
       <c r="D6" s="3">
-        <v>0</v>
+        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!J4/'Data from BNVP'!$E$5)</f>
+        <v>3076.1462883723043</v>
       </c>
       <c r="E6" s="3">
-        <f>$E$3*('Data from BNVP'!K5/'Data from BNVP'!$E$5)</f>
-        <v>1025382.0961241014</v>
+        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!J5/'Data from BNVP'!$E$5)</f>
+        <v>3076.1462883723043</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -9667,8 +10155,8 @@
         <v>0</v>
       </c>
       <c r="H6" s="3">
-        <f>$E$3*('Data from BNVP'!K8/'Data from BNVP'!$E$5)</f>
-        <v>2379662.8831780958</v>
+        <f>'SDoVPbT-frgt'!$E$3*('Data from BNVP'!J8/'Data from BNVP'!$E$5)</f>
+        <v>7138.988649534288</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.45">
@@ -9676,31 +10164,26 @@
         <v>13</v>
       </c>
       <c r="B7" s="3">
-        <f>'SDoVPbT-psgr'!B7</f>
+        <f>D7*('Data from BNVP'!L2/'Data from BNVP'!L4)</f>
         <v>7615.0170715103632</v>
       </c>
-      <c r="C7" s="3">
-        <f>D7</f>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="18">
+        <f>Calculations!B4</f>
         <v>4633.1654645849012</v>
       </c>
-      <c r="D7" s="3">
-        <f>'SDoVPbT-psgr'!D7</f>
-        <v>4633.1654645849012</v>
-      </c>
-      <c r="E7" s="3">
-        <f>D7</f>
-        <v>4633.1654645849012</v>
-      </c>
-      <c r="F7" s="3">
-        <f>'SDoVPbT-psgr'!F7</f>
+      <c r="E7">
         <v>0</v>
       </c>
-      <c r="G7" s="3">
-        <f>E7</f>
-        <v>4633.1654645849012</v>
-      </c>
-      <c r="H7" s="3">
-        <f>'SDoVPbT-psgr'!H7</f>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>0</v>
       </c>
     </row>

</xml_diff>